<commit_message>
Finished simple light map. (only applied to first directional light now)
</commit_message>
<xml_diff>
--- a/Graphics II Project Rubric.xlsx
+++ b/Graphics II Project Rubric.xlsx
@@ -233,7 +233,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="82">
   <si>
     <t>Apply a post process routine via pixel shader (eg Blur or Custom Pixel Maipulations)</t>
   </si>
@@ -528,6 +528,9 @@
   </si>
   <si>
     <t>X</t>
+  </si>
+  <si>
+    <t>II</t>
   </si>
 </sst>
 </file>
@@ -1051,8 +1054,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1184,7 +1187,7 @@
       </c>
       <c r="I4" s="5">
         <f>IF(SUMIF(E4:E85,"=II",G4:G85) + SUMIF(D90:D91, "X",B90:B91) &gt; 22, 22, SUMIF(E4:E85,"=II",G4:G85) + SUMIF(D90:D91, "X",B90:B91))</f>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="J4" s="5">
         <f>IF(SUMIF(E4:E85,"=III",G4:G85) + SUMIF(E90:E91, "X",B90:B91) &gt; 22, 22, SUMIF(E4:E85,"=III",G4:G85) + SUMIF(E90:E91, "X",B90:B91))</f>
@@ -1196,7 +1199,7 @@
       </c>
       <c r="L4" s="9">
         <f>SUM(G4:G85) + SUMIF(C90:C91, "X",B90:B91) + SUMIF(D90:D91, "X",B90:B91) + SUMIF(E90:E91, "X",B90:B91)</f>
-        <v>67</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
@@ -1249,11 +1252,15 @@
       <c r="D6" s="5">
         <v>5</v>
       </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="3"/>
+      <c r="E6" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>80</v>
+      </c>
       <c r="G6" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H6" s="5">
         <f>IF(SUMIF(E4:E85,"=I",G4:G85) + SUMIF(C90:C91, "X",B90:B91)  &gt; 22, SUMIF(E4:E85,"=I",G4:G85) + SUMIF(C90:C91, "X",B90:B91) - 22,0)</f>
@@ -1270,7 +1277,7 @@
       <c r="K6" s="5"/>
       <c r="L6" s="9">
         <f>IF(L4 &gt; 66, SUM(-66,L4),0)</f>
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
@@ -1394,11 +1401,11 @@
       </c>
       <c r="I10" s="5">
         <f>IF(H10+I4 - 22 &gt; 0, H10+I4 - 22, 0)</f>
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="J10" s="5">
         <f>IF(I10+J4 - 22 &gt; 0, I10+J4 - 22, 0)</f>
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
@@ -1628,11 +1635,15 @@
       <c r="D21" s="5">
         <v>3</v>
       </c>
-      <c r="E21" s="2"/>
-      <c r="F21" s="3"/>
+      <c r="E21" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>80</v>
+      </c>
       <c r="G21" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H21" s="5"/>
       <c r="I21" s="5"/>
@@ -2051,11 +2062,15 @@
       <c r="D38" s="5">
         <v>3</v>
       </c>
-      <c r="E38" s="2"/>
-      <c r="F38" s="3"/>
+      <c r="E38" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>80</v>
+      </c>
       <c r="G38" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H38" s="5"/>
       <c r="I38" s="5"/>

</xml_diff>

<commit_message>
Add post processing effect, gamma correction. Update rubric.
</commit_message>
<xml_diff>
--- a/Graphics II Project Rubric.xlsx
+++ b/Graphics II Project Rubric.xlsx
@@ -305,7 +305,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="83">
   <si>
     <t>Apply a post process routine via pixel shader (eg Blur or Custom Pixel Maipulations)</t>
   </si>
@@ -1129,8 +1129,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="B52" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F76" sqref="F76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1266,15 +1266,15 @@
       </c>
       <c r="J4" s="5">
         <f>IF(SUMIF(E4:E85,"=III",G4:G85) + SUMIF(E90:E91, "X",B90:B91) &gt; 22, 22, SUMIF(E4:E85,"=III",G4:G85) + SUMIF(E90:E91, "X",B90:B91))</f>
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="K4" s="5">
         <f>SUM(H6,I6,J6)</f>
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="L4" s="9">
         <f>SUM(G4:G85) + SUMIF(C90:C91, "X",B90:B91) + SUMIF(D90:D91, "X",B90:B91) + SUMIF(E90:E91, "X",B90:B91)</f>
-        <v>116</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
@@ -1347,12 +1347,12 @@
       </c>
       <c r="J6" s="5">
         <f>IF(SUMIF(E4:E85,"=III",G4:G85) + SUMIF(E90:E91, "X",B90:B91) &gt; 22, SUMIF(E4:E85,"=III",G4:G85) + SUMIF(E90:E91, "X",B90:B91) - 22,0)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="K6" s="5"/>
       <c r="L6" s="9">
         <f>IF(L4 &gt; 66, SUM(-66,L4),0)</f>
-        <v>50</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
@@ -1480,15 +1480,15 @@
       </c>
       <c r="H10" s="5">
         <f>IF(K4+H4 - 22 &gt; 0, K4+H4 - 22, 0)</f>
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="I10" s="5">
         <f>IF(H10+I4 - 22 &gt; 0, H10+I4 - 22, 0)</f>
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="J10" s="5">
         <f>IF(I10+J4 - 22 &gt; 0, I10+J4 - 22, 0)</f>
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
@@ -2813,11 +2813,15 @@
       <c r="D68" s="5">
         <v>5</v>
       </c>
-      <c r="E68" s="2"/>
-      <c r="F68" s="3"/>
+      <c r="E68" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="F68" s="3" t="s">
+        <v>80</v>
+      </c>
       <c r="G68" s="8">
         <f t="shared" ref="G68:G85" si="2" xml:space="preserve"> IF(EXACT(F68,"X"),IF(EXACT(E68,"I"),$B68,IF(EXACT(E68,"II"),$C68,IF(EXACT(E68,"III"),$D68,0))),0)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H68" s="5"/>
       <c r="I68" s="5"/>
@@ -2942,11 +2946,15 @@
       <c r="D75" s="5">
         <v>5</v>
       </c>
-      <c r="E75" s="2"/>
-      <c r="F75" s="3"/>
+      <c r="E75" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="F75" s="3" t="s">
+        <v>80</v>
+      </c>
       <c r="G75" s="8">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H75" s="5"/>
       <c r="I75" s="5"/>

</xml_diff>

<commit_message>
Add key control to different post processing effects.
</commit_message>
<xml_diff>
--- a/Graphics II Project Rubric.xlsx
+++ b/Graphics II Project Rubric.xlsx
@@ -248,6 +248,30 @@
           </rPr>
           <t xml:space="preserve">
 Requires Camera Movement</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E75" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Press '4' for gamma correction, '5' for edge detection and '6' to turn off post processing effect.</t>
         </r>
       </text>
     </comment>
@@ -1129,8 +1153,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B52" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F76" sqref="F76"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E75" sqref="E75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3374,7 +3398,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6 K4 H6:J6">
+  <conditionalFormatting sqref="K4 L6 H6:J6">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>